<commit_message>
Changed url from stage to prod
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/ProductListPage.xlsx
+++ b/src/test/java/com/born/xls/ProductListPage.xlsx
@@ -2025,8 +2025,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K682"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C151" sqref="C151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>